<commit_message>
Kris modifications to metrics.xlsx (correct sorting in chart)
</commit_message>
<xml_diff>
--- a/data/robots/reflex/results/160215_graphs/metrics.xlsx
+++ b/data/robots/reflex/results/160215_graphs/metrics.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arocchi\Desktop\ssoch\log\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,7 +213,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -319,7 +314,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -389,7 +384,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2C14-4EC2-8954-7B827B4E8E05}"/>
             </c:ext>
@@ -445,7 +440,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2C14-4EC2-8954-7B827B4E8E05}"/>
             </c:ext>
@@ -501,7 +496,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-2C14-4EC2-8954-7B827B4E8E05}"/>
             </c:ext>
@@ -516,11 +511,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="149462528"/>
-        <c:axId val="371935488"/>
+        <c:axId val="9007616"/>
+        <c:axId val="8937472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149462528"/>
+        <c:axId val="9007616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="371935488"/>
+        <c:crossAx val="8937472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -538,7 +533,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="371935488"/>
+        <c:axId val="8937472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +544,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149462528"/>
+        <c:crossAx val="9007616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -572,7 +567,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -642,7 +637,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FF64-4E93-A534-263789661406}"/>
             </c:ext>
@@ -698,7 +693,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FF64-4E93-A534-263789661406}"/>
             </c:ext>
@@ -713,11 +708,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="148716032"/>
-        <c:axId val="175435712"/>
+        <c:axId val="9008640"/>
+        <c:axId val="8939776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="148716032"/>
+        <c:axId val="9008640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -727,7 +722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175435712"/>
+        <c:crossAx val="8939776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -735,7 +730,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175435712"/>
+        <c:axId val="8939776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,7 +741,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148716032"/>
+        <c:crossAx val="9008640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -769,7 +764,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -927,7 +922,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1579-4923-BCD7-2AFFD75B7886}"/>
             </c:ext>
@@ -1061,7 +1056,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1579-4923-BCD7-2AFFD75B7886}"/>
             </c:ext>
@@ -1076,13 +1071,13 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="148717056"/>
-        <c:axId val="362975168"/>
+        <c:axId val="9009152"/>
+        <c:axId val="8942080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="148717056"/>
+        <c:axId val="9009152"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1100,7 +1095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362975168"/>
+        <c:crossAx val="8942080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1108,7 +1103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362975168"/>
+        <c:axId val="8942080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,8 +1133,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148717056"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="9009152"/>
+        <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -1161,7 +1156,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1319,7 +1314,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E340-42B5-962B-986C88EFF54D}"/>
             </c:ext>
@@ -1453,7 +1448,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E340-42B5-962B-986C88EFF54D}"/>
             </c:ext>
@@ -1468,13 +1463,13 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="258643456"/>
-        <c:axId val="257046720"/>
+        <c:axId val="9009664"/>
+        <c:axId val="8944384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="258643456"/>
+        <c:axId val="9009664"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1492,7 +1487,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257046720"/>
+        <c:crossAx val="8944384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1500,7 +1495,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257046720"/>
+        <c:axId val="8944384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1530,8 +1525,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="258643456"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="9009664"/>
+        <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -1553,7 +1548,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1711,7 +1706,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DFA2-464C-9C43-5D72FE19B69F}"/>
             </c:ext>
@@ -1845,7 +1840,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DFA2-464C-9C43-5D72FE19B69F}"/>
             </c:ext>
@@ -1860,13 +1855,13 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="257249280"/>
-        <c:axId val="257632512"/>
+        <c:axId val="9010176"/>
+        <c:axId val="181683328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="257249280"/>
+        <c:axId val="9010176"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1884,7 +1879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257632512"/>
+        <c:crossAx val="181683328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1892,7 +1887,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257632512"/>
+        <c:axId val="181683328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1922,8 +1917,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257249280"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="9010176"/>
+        <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -2146,7 +2141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2181,7 +2176,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2392,8 +2387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" topLeftCell="I26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>